<commit_message>
Update pinout with correction for 2.0 enable pin
Update pinout with correction for 2.0 enable pin thanks Aaryn
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="342">
   <si>
     <t>Name</t>
   </si>
@@ -1060,6 +1060,9 @@
   </si>
   <si>
     <t>Extruder 2 filament  sensor, 1 = empty</t>
+  </si>
+  <si>
+    <t>Motor E2 enable, 0 = enable</t>
   </si>
 </sst>
 </file>
@@ -1984,8 +1987,8 @@
   </sheetPr>
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D130" sqref="D130"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,6 +3371,12 @@
       <c r="C65">
         <v>141</v>
       </c>
+      <c r="D65">
+        <v>128</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">

</xml_diff>

<commit_message>
Update pinout for Top Cover
Update pinout for Top Cover
input pin  6 : Top cover sensor
0 = open
1=close
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -118,15 +118,9 @@
     <t>PC24</t>
   </si>
   <si>
-    <t>Top cover sensor, 1 = open</t>
-  </si>
-  <si>
     <t>input</t>
   </si>
   <si>
-    <t>PC24,135,6,"Top cover sensor, 1 = open",In</t>
-  </si>
-  <si>
     <t>PC23</t>
   </si>
   <si>
@@ -1046,6 +1040,12 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Top cover sensor, 0 = open 1=close</t>
+  </si>
+  <si>
+    <t>PC24,135,6,"Top cover sensor,  0 = open 1=close</t>
   </si>
 </sst>
 </file>
@@ -1607,8 +1607,8 @@
   </sheetPr>
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H1:H2"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,15 +1645,15 @@
         <v>5</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C2" s="11">
         <v>121</v>
@@ -1662,13 +1662,13 @@
         <v>121</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H2" s="18">
         <v>14</v>
@@ -1676,10 +1676,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C3" s="11">
         <v>122</v>
@@ -1688,13 +1688,13 @@
         <v>122</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H3" s="18">
         <v>14</v>
@@ -1702,10 +1702,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C4" s="11">
         <v>123</v>
@@ -1714,13 +1714,13 @@
         <v>123</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H4" s="18">
         <v>14</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C5" s="22">
         <v>118</v>
@@ -1740,13 +1740,13 @@
         <v>118</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H5" s="18">
         <v>13</v>
@@ -1754,10 +1754,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C6" s="22">
         <v>119</v>
@@ -1766,13 +1766,13 @@
         <v>119</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H6" s="18">
         <v>13</v>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C7" s="22">
         <v>120</v>
@@ -1792,13 +1792,13 @@
         <v>120</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H7" s="18">
         <v>13</v>
@@ -1806,10 +1806,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C8" s="22">
         <v>2</v>
@@ -1818,13 +1818,13 @@
         <v>124</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H8" s="17">
         <v>13</v>
@@ -1832,10 +1832,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C9" s="14">
         <v>142</v>
@@ -1844,13 +1844,13 @@
         <v>78</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>245</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>247</v>
       </c>
       <c r="H9" s="18">
         <v>12</v>
@@ -1858,10 +1858,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C10" s="14">
         <v>129</v>
@@ -1870,13 +1870,13 @@
         <v>85</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H10" s="18">
         <v>12</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="12">
         <v>71</v>
@@ -1896,13 +1896,13 @@
         <v>42</v>
       </c>
       <c r="E11" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>160</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>162</v>
       </c>
       <c r="H11" s="18">
         <v>11</v>
@@ -1910,10 +1910,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" s="12">
         <v>72</v>
@@ -1922,13 +1922,13 @@
         <v>43</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H12" s="18">
         <v>11</v>
@@ -1936,10 +1936,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C13" s="12">
         <v>79</v>
@@ -1948,13 +1948,13 @@
         <v>55</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H13" s="18">
         <v>11</v>
@@ -1962,10 +1962,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C14" s="12">
         <v>80</v>
@@ -1974,13 +1974,13 @@
         <v>56</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H14" s="18">
         <v>11</v>
@@ -1988,10 +1988,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C15" s="12">
         <v>81</v>
@@ -2000,13 +2000,13 @@
         <v>57</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H15" s="18">
         <v>11</v>
@@ -2014,10 +2014,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C16" s="12">
         <v>107</v>
@@ -2026,13 +2026,13 @@
         <v>73</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H16" s="18">
         <v>11</v>
@@ -2040,10 +2040,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C17" s="12">
         <v>108</v>
@@ -2052,13 +2052,13 @@
         <v>74</v>
       </c>
       <c r="E17" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>232</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>234</v>
       </c>
       <c r="H17" s="18">
         <v>11</v>
@@ -2066,10 +2066,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="7">
         <v>133</v>
@@ -2078,13 +2078,13 @@
         <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="H18" s="18">
         <v>10</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="7">
         <v>68</v>
@@ -2104,7 +2104,7 @@
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>18</v>
@@ -2116,10 +2116,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C20" s="7">
         <v>59</v>
@@ -2128,13 +2128,13 @@
         <v>34</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="H20" s="18">
         <v>10</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" s="7">
         <v>60</v>
@@ -2154,13 +2154,13 @@
         <v>35</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="H21" s="18">
         <v>10</v>
@@ -2168,10 +2168,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C22" s="7">
         <v>116</v>
@@ -2180,13 +2180,13 @@
         <v>36</v>
       </c>
       <c r="E22" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="H22" s="18">
         <v>10</v>
@@ -2194,10 +2194,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C23" s="7">
         <v>63</v>
@@ -2206,13 +2206,13 @@
         <v>37</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="H23" s="18">
         <v>10</v>
@@ -2220,10 +2220,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C24" s="7">
         <v>64</v>
@@ -2232,13 +2232,13 @@
         <v>38</v>
       </c>
       <c r="E24" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="H24" s="18">
         <v>10</v>
@@ -2246,10 +2246,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C25" s="7">
         <v>65</v>
@@ -2258,13 +2258,13 @@
         <v>39</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="H25" s="18">
         <v>10</v>
@@ -2272,10 +2272,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C26" s="7">
         <v>66</v>
@@ -2284,13 +2284,13 @@
         <v>40</v>
       </c>
       <c r="E26" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="H26" s="18">
         <v>10</v>
@@ -2298,10 +2298,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C27" s="7">
         <v>67</v>
@@ -2310,13 +2310,13 @@
         <v>41</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="H27" s="18">
         <v>10</v>
@@ -2324,10 +2324,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C28" s="7">
         <v>143</v>
@@ -2336,13 +2336,13 @@
         <v>125</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>304</v>
       </c>
       <c r="H28" s="17">
         <v>10</v>
@@ -2350,10 +2350,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" s="11">
         <v>6</v>
@@ -2362,13 +2362,13 @@
         <v>16</v>
       </c>
       <c r="E29" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="H29" s="18">
         <v>9</v>
@@ -2376,10 +2376,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" s="11">
         <v>8</v>
@@ -2388,13 +2388,13 @@
         <v>24</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H30" s="18">
         <v>9</v>
@@ -2402,10 +2402,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31" s="11">
         <v>13</v>
@@ -2414,13 +2414,13 @@
         <v>25</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>26</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H31" s="18">
         <v>9</v>
@@ -2428,10 +2428,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C32" s="11">
         <v>91</v>
@@ -2440,13 +2440,13 @@
         <v>65</v>
       </c>
       <c r="E32" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>203</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="H32" s="18">
         <v>9</v>
@@ -2454,10 +2454,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C33" s="10">
         <v>21</v>
@@ -2466,13 +2466,13 @@
         <v>12</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H33" s="18">
         <v>8</v>
@@ -2480,10 +2480,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="10">
         <v>22</v>
@@ -2492,13 +2492,13 @@
         <v>30</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H34" s="18">
         <v>8</v>
@@ -2506,10 +2506,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C35" s="10">
         <v>24</v>
@@ -2518,13 +2518,13 @@
         <v>68</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H35" s="18">
         <v>8</v>
@@ -2532,10 +2532,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C36" s="10">
         <v>23</v>
@@ -2544,13 +2544,13 @@
         <v>69</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H36" s="18">
         <v>8</v>
@@ -2558,10 +2558,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C37" s="9">
         <v>20</v>
@@ -2570,13 +2570,13 @@
         <v>11</v>
       </c>
       <c r="E37" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="H37" s="18">
         <v>7</v>
@@ -2584,10 +2584,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C38" s="9">
         <v>17</v>
@@ -2596,13 +2596,13 @@
         <v>14</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H38" s="18">
         <v>7</v>
@@ -2610,10 +2610,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="9">
         <v>18</v>
@@ -2622,13 +2622,13 @@
         <v>15</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H39" s="18">
         <v>7</v>
@@ -2636,10 +2636,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C40" s="9">
         <v>19</v>
@@ -2648,13 +2648,13 @@
         <v>29</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H40" s="18">
         <v>7</v>
@@ -2662,10 +2662,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="8">
         <v>102</v>
@@ -2674,13 +2674,13 @@
         <v>10</v>
       </c>
       <c r="E41" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="H41" s="18">
         <v>6</v>
@@ -2688,10 +2688,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C42" s="8">
         <v>101</v>
@@ -2700,13 +2700,13 @@
         <v>44</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H42" s="18">
         <v>6</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C43" s="8">
         <v>103</v>
@@ -2726,13 +2726,13 @@
         <v>72</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H43" s="18">
         <v>6</v>
@@ -2740,10 +2740,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C44" s="8">
         <v>109</v>
@@ -2752,13 +2752,13 @@
         <v>75</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H44" s="18">
         <v>6</v>
@@ -2766,10 +2766,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C45" s="8">
         <v>110</v>
@@ -2778,13 +2778,13 @@
         <v>76</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H45" s="18">
         <v>6</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C46" s="8">
         <v>111</v>
@@ -2804,13 +2804,13 @@
         <v>77</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H46" s="18">
         <v>6</v>
@@ -2830,13 +2830,13 @@
         <v>6</v>
       </c>
       <c r="E47" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G47" s="5" t="s">
-        <v>35</v>
+        <v>342</v>
       </c>
       <c r="H47" s="18">
         <v>4</v>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C48" s="5">
         <v>134</v>
@@ -2856,13 +2856,13 @@
         <v>7</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H48" s="20">
         <v>4</v>
@@ -2870,10 +2870,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C49" s="5">
         <v>7</v>
@@ -2882,13 +2882,13 @@
         <v>23</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H49" s="18">
         <v>4</v>
@@ -2896,10 +2896,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C50" s="5">
         <v>9</v>
@@ -2908,13 +2908,13 @@
         <v>70</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H50" s="18">
         <v>4</v>
@@ -2922,10 +2922,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C51" s="21">
         <v>113</v>
@@ -2934,13 +2934,13 @@
         <v>115</v>
       </c>
       <c r="E51" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="G51" s="21" t="s">
         <v>262</v>
-      </c>
-      <c r="F51" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="G51" s="21" t="s">
-        <v>264</v>
       </c>
       <c r="H51" s="18">
         <v>4</v>
@@ -2948,10 +2948,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C52" s="21">
         <v>114</v>
@@ -2960,13 +2960,13 @@
         <v>116</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H52" s="18">
         <v>4</v>
@@ -3000,10 +3000,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C54" s="4">
         <v>5</v>
@@ -3012,13 +3012,13 @@
         <v>17</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H54" s="18">
         <v>3</v>
@@ -3026,10 +3026,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C55" s="4">
         <v>115</v>
@@ -3041,10 +3041,10 @@
         <v>29</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H55" s="18">
         <v>3</v>
@@ -3052,25 +3052,25 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C56" s="4">
         <v>92</v>
       </c>
       <c r="D56" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="G56" s="4" t="s">
         <v>313</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>315</v>
       </c>
       <c r="H56" s="17">
         <v>3</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C59" s="3">
         <v>86</v>
@@ -3140,13 +3140,13 @@
         <v>20</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H59" s="18">
         <v>2</v>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C60" s="3">
         <v>140</v>
@@ -3166,13 +3166,13 @@
         <v>53</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H60" s="18">
         <v>2</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3">
@@ -3190,7 +3190,7 @@
         <v>128</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C62" s="3">
         <v>128</v>
@@ -3212,13 +3212,13 @@
         <v>129</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H62" s="17">
         <v>2</v>
@@ -3226,25 +3226,25 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C63" s="3">
         <v>89</v>
       </c>
       <c r="D63" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G63" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="H63" s="17">
         <v>2</v>
@@ -3326,10 +3326,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C67" s="2">
         <v>132</v>
@@ -3338,7 +3338,7 @@
         <v>9</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="19"/>
@@ -3348,10 +3348,10 @@
     </row>
     <row r="68" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C68" s="2">
         <v>4</v>
@@ -3360,7 +3360,7 @@
         <v>18</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="19"/>
@@ -3370,10 +3370,10 @@
     </row>
     <row r="69" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C69" s="2">
         <v>3</v>
@@ -3382,7 +3382,7 @@
         <v>19</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="19"/>
@@ -3392,10 +3392,10 @@
     </row>
     <row r="70" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C70" s="2">
         <v>87</v>
@@ -3404,7 +3404,7 @@
         <v>21</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="19"/>
@@ -3414,10 +3414,10 @@
     </row>
     <row r="71" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C71" s="2">
         <v>1</v>
@@ -3426,7 +3426,7 @@
         <v>22</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>18</v>
@@ -3438,10 +3438,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C72" s="2">
         <v>14</v>
@@ -3450,7 +3450,7 @@
         <v>26</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="19"/>
@@ -3460,10 +3460,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C73" s="2">
         <v>15</v>
@@ -3472,7 +3472,7 @@
         <v>27</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="19"/>
@@ -3482,10 +3482,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C74" s="2">
         <v>16</v>
@@ -3494,7 +3494,7 @@
         <v>28</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="19"/>
@@ -3504,10 +3504,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C75" s="2">
         <v>26</v>
@@ -3516,13 +3516,13 @@
         <v>31</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H75" s="18">
         <v>0</v>
@@ -3530,10 +3530,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C76" s="2">
         <v>32</v>
@@ -3542,7 +3542,7 @@
         <v>32</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="19"/>
@@ -3552,10 +3552,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C77" s="2">
         <v>55</v>
@@ -3564,7 +3564,7 @@
         <v>33</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>18</v>
@@ -3576,10 +3576,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C78" s="2">
         <v>100</v>
@@ -3588,13 +3588,13 @@
         <v>45</v>
       </c>
       <c r="E78" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G78" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G78" s="19" t="s">
-        <v>172</v>
       </c>
       <c r="H78" s="18">
         <v>0</v>
@@ -3602,10 +3602,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C79" s="2">
         <v>99</v>
@@ -3614,7 +3614,7 @@
         <v>46</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="19"/>
@@ -3624,10 +3624,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C80" s="2">
         <v>98</v>
@@ -3636,7 +3636,7 @@
         <v>47</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="19"/>
@@ -3646,10 +3646,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C81" s="2">
         <v>97</v>
@@ -3658,7 +3658,7 @@
         <v>48</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="19"/>
@@ -3668,10 +3668,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C82" s="2">
         <v>96</v>
@@ -3680,7 +3680,7 @@
         <v>49</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="19"/>
@@ -3690,10 +3690,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C83" s="2">
         <v>95</v>
@@ -3702,7 +3702,7 @@
         <v>50</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="19"/>
@@ -3712,10 +3712,10 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C84" s="2">
         <v>94</v>
@@ -3724,7 +3724,7 @@
         <v>51</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="19"/>
@@ -3762,10 +3762,10 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C87" s="2">
         <v>82</v>
@@ -3774,13 +3774,13 @@
         <v>58</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G87" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H87" s="18">
         <v>0</v>
@@ -3872,10 +3872,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C94" s="2">
         <v>76</v>
@@ -3884,13 +3884,13 @@
         <v>66</v>
       </c>
       <c r="E94" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G94" s="19" t="s">
         <v>207</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G94" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="H94" s="18">
         <v>0</v>
@@ -3898,10 +3898,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C95" s="2">
         <v>77</v>
@@ -3910,10 +3910,10 @@
         <v>67</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G95" s="19"/>
       <c r="H95" s="18">
@@ -3922,10 +3922,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C96" s="2">
         <v>70</v>
@@ -4049,10 +4049,10 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C104" s="2">
         <v>112</v>
@@ -4061,13 +4061,13 @@
         <v>87</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G104" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H104" s="18">
         <v>0</v>
@@ -4243,10 +4243,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C117" s="2">
         <v>25</v>
@@ -4256,10 +4256,10 @@
       </c>
       <c r="E117" s="2"/>
       <c r="F117" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G117" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H117" s="18">
         <v>0</v>
@@ -4267,7 +4267,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="2">
@@ -4327,7 +4327,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="2">
@@ -4389,7 +4389,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="2">
@@ -4491,16 +4491,16 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C133" s="2">
         <v>78</v>
       </c>
       <c r="D133" s="24" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
@@ -4511,20 +4511,20 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C134" s="2">
         <v>90</v>
       </c>
       <c r="D134" s="24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G134" s="2"/>
       <c r="H134" s="17">
@@ -4533,16 +4533,16 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C135" s="2">
         <v>83</v>
       </c>
       <c r="D135" s="24" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
@@ -4553,16 +4553,16 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C136" s="2">
         <v>84</v>
       </c>
       <c r="D136" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
@@ -4573,16 +4573,16 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C137" s="2">
         <v>85</v>
       </c>
       <c r="D137" s="24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
@@ -4593,20 +4593,20 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C138" s="2">
         <v>88</v>
       </c>
       <c r="D138" s="24" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G138" s="2"/>
       <c r="H138" s="17">
@@ -4615,10 +4615,10 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C139" s="2">
         <v>28</v>
@@ -4633,10 +4633,10 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C140" s="2">
         <v>29</v>
@@ -4651,10 +4651,10 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C141" s="2">
         <v>30</v>
@@ -4669,10 +4669,10 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C142" s="2">
         <v>31</v>
@@ -4687,7 +4687,7 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="2">
@@ -4703,10 +4703,10 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C144" s="2">
         <v>130</v>

</xml_diff>

<commit_message>
Add pins for Jam sensor
Add pins for Jam sensor
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="345">
   <si>
     <t>Name</t>
   </si>
@@ -1046,6 +1046,12 @@
   </si>
   <si>
     <t>PC24,135,6,"Top cover sensor,  0 = open 1=close</t>
+  </si>
+  <si>
+    <t>Right Jam Sensor (0 = black; 1=reflect)</t>
+  </si>
+  <si>
+    <t>Left Jam Sensor (0 = black; 1=reflect)</t>
   </si>
 </sst>
 </file>
@@ -1607,8 +1613,8 @@
   </sheetPr>
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2908,7 +2914,7 @@
         <v>70</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>35</v>
+        <v>343</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>51</v>
@@ -4398,11 +4404,15 @@
       <c r="D126" s="2">
         <v>108</v>
       </c>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
+      <c r="E126" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="G126" s="2"/>
       <c r="H126" s="18">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>